<commit_message>
FIX: Corregida actualización de Variación promedio anual en paso 5 sectorial
</commit_message>
<xml_diff>
--- a/applications/formularios_sectoriales/Clasificador_Presupuestario.xlsx
+++ b/applications/formularios_sectoriales/Clasificador_Presupuestario.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peaton\Documents\Trabajo\desarrollo\Transferencia_de_Competencias\back\applications\formularios_sectoriales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaime\Desktop\SUBDERE\Transferencia de Competencias\transferenciacompetencias\applications\formularios_sectoriales\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D02911-2E9A-409F-8F4E-D7BA02A80A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="2" r:id="rId1"/>
@@ -19,17 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -307,7 +297,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -624,11 +614,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>